<commit_message>
Update on 20200330 part 2
</commit_message>
<xml_diff>
--- a/文档/测试工作相关/IT端到端测试相关/测试内容相关/2019/20191209/12.10上仿真端到端测试记录.xlsx
+++ b/文档/测试工作相关/IT端到端测试相关/测试内容相关/2019/20191209/12.10上仿真端到端测试记录.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="7140" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="18525" windowHeight="7140"/>
   </bookViews>
   <sheets>
     <sheet name="测试概览" sheetId="5" r:id="rId1"/>
@@ -12,8 +12,8 @@
     <sheet name="BUG汇总 " sheetId="8" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">测试案例!$I$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'BUG汇总 '!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">测试案例!$H$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">测试概览!$A$1:$H$4</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
   <si>
     <t>序号</t>
   </si>
@@ -127,18 +127,12 @@
 2.派发客保工单时验证工单报文含有“是否发起工程建设”</t>
   </si>
   <si>
-    <t>李栋</t>
-  </si>
-  <si>
     <t>1.登陆新CRM系统受理专线宽带新装单，订单结算后提交。
 2.IBP收到CRM订单后发送创服务给综资，并且等待配置。
 3.综资收到订单后自动配置并提交
 4.IBP收到资源信息后派发客保工单</t>
   </si>
   <si>
-    <t>张轶晟</t>
-  </si>
-  <si>
     <t>1.登陆新CRM系统使用已有资产受理有线宽带修改单，修改速率后订单结算后提交。
 2.IBP收到CRM订单发送综资原资产查询，获取原资产信息后发送创服务并等待综资配置
 3.综资收到订单后自动配置并提交
@@ -172,14 +166,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="21">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,151 +184,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -353,194 +203,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="13">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -600,255 +264,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="18" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -885,144 +307,79 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
   <colors>
     <mruColors>
-      <color rgb="00808080"/>
-      <color rgb="0000B050"/>
+      <color rgb="FF808080"/>
+      <color rgb="FF00B050"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1312,147 +669,145 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="6.33636363636364" style="29" customWidth="1"/>
-    <col min="2" max="2" width="17" style="29" customWidth="1"/>
-    <col min="3" max="3" width="23.2727272727273" style="29" customWidth="1"/>
-    <col min="4" max="4" width="13.2181818181818" style="29" customWidth="1"/>
-    <col min="5" max="5" width="7.18181818181818" style="29" customWidth="1"/>
-    <col min="6" max="6" width="9.09090909090909" style="29" customWidth="1"/>
-    <col min="7" max="7" width="12.1818181818182" style="29" customWidth="1"/>
-    <col min="8" max="8" width="12.6272727272727" style="30"/>
-    <col min="9" max="16384" width="9" style="29"/>
+    <col min="1" max="1" width="6.375" style="17" customWidth="1"/>
+    <col min="2" max="2" width="17" style="17" customWidth="1"/>
+    <col min="3" max="3" width="23.25" style="17" customWidth="1"/>
+    <col min="4" max="4" width="13.25" style="17" customWidth="1"/>
+    <col min="5" max="5" width="7.125" style="17" customWidth="1"/>
+    <col min="6" max="6" width="9.125" style="17" customWidth="1"/>
+    <col min="7" max="7" width="12.125" style="17" customWidth="1"/>
+    <col min="8" max="8" width="12.625" style="18"/>
+    <col min="9" max="16384" width="9" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" s="29" customFormat="1" spans="1:10">
-      <c r="A1" s="31" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="31" t="s">
+      <c r="D1" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="31" t="s">
+      <c r="E1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="32" t="s">
+      <c r="G1" s="20" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="I1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="38"/>
-    </row>
-    <row r="2" s="29" customFormat="1" ht="56" spans="1:9">
-      <c r="A2" s="14">
+      <c r="J1" s="26"/>
+    </row>
+    <row r="2" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A2" s="12">
         <v>1</v>
       </c>
-      <c r="B2" s="14">
+      <c r="B2" s="12">
         <v>196058868</v>
       </c>
-      <c r="C2" s="14" t="s">
+      <c r="C2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="34"/>
-      <c r="E2" s="35">
+      <c r="D2" s="22"/>
+      <c r="E2" s="23">
         <v>3</v>
       </c>
-      <c r="F2" s="35"/>
-      <c r="G2" s="36"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="14"/>
-    </row>
-    <row r="3" ht="56" spans="1:9">
-      <c r="A3" s="14">
+      <c r="F2" s="23"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="12"/>
+    </row>
+    <row r="3" spans="1:10" ht="40.5" x14ac:dyDescent="0.15">
+      <c r="A3" s="12">
         <v>2</v>
       </c>
-      <c r="B3" s="14">
+      <c r="B3" s="12">
         <v>196110130</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="34" t="s">
+      <c r="D3" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="35">
+      <c r="E3" s="23">
         <v>4</v>
       </c>
-      <c r="F3" s="35"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="14"/>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="14">
+      <c r="F3" s="23"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="12"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+      <c r="A4" s="12">
         <v>3</v>
       </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="35"/>
-      <c r="F4" s="35"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="37"/>
-      <c r="I4" s="14"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="12"/>
     </row>
   </sheetData>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:L8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="7"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="8.36363636363636" customWidth="1"/>
-    <col min="2" max="2" width="13.7272727272727" style="1" customWidth="1"/>
-    <col min="3" max="3" width="38.4545454545455" style="4" customWidth="1"/>
-    <col min="4" max="4" width="35.7272727272727" style="4" customWidth="1"/>
+    <col min="1" max="1" width="8.375" customWidth="1"/>
+    <col min="2" max="2" width="13.75" style="1" customWidth="1"/>
+    <col min="3" max="3" width="38.5" style="4" customWidth="1"/>
+    <col min="4" max="4" width="35.75" style="4" customWidth="1"/>
     <col min="5" max="5" width="33" style="4" customWidth="1"/>
-    <col min="6" max="6" width="10.0909090909091" customWidth="1"/>
-    <col min="7" max="7" width="8.18181818181818" customWidth="1"/>
-    <col min="8" max="8" width="10.4545454545455" customWidth="1"/>
-    <col min="9" max="9" width="12.6363636363636" customWidth="1"/>
-    <col min="10" max="10" width="21.2727272727273" style="4" customWidth="1"/>
-    <col min="11" max="11" width="10.5454545454545" customWidth="1"/>
-    <col min="12" max="12" width="11.6363636363636" style="4" customWidth="1"/>
+    <col min="6" max="6" width="10.125" customWidth="1"/>
+    <col min="7" max="7" width="10.5" customWidth="1"/>
+    <col min="8" max="8" width="12.625" customWidth="1"/>
+    <col min="9" max="9" width="21.25" style="4" customWidth="1"/>
+    <col min="10" max="10" width="10.5" customWidth="1"/>
+    <col min="11" max="11" width="11.625" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="9" customFormat="1" ht="25" customHeight="1" spans="1:12">
+    <row r="1" spans="1:11" s="9" customFormat="1" ht="24.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -1471,222 +826,201 @@
       <c r="F1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="11" t="s">
+      <c r="G1" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="H1" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="28" t="s">
+      <c r="I1" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="K1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="K1" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" ht="175" customHeight="1" spans="1:12">
+    <row r="2" spans="1:11" ht="174.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="8">
         <v>1</v>
       </c>
-      <c r="B2" s="12">
+      <c r="B2" s="27">
         <v>196058868</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="12" t="s">
         <v>21</v>
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="17"/>
-    </row>
-    <row r="3" ht="168" customHeight="1" spans="1:12">
+      <c r="I2" s="13"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="13"/>
+    </row>
+    <row r="3" spans="1:11" ht="168" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="8">
         <v>2</v>
       </c>
-      <c r="B3" s="15"/>
-      <c r="C3" s="16"/>
-      <c r="D3" s="14" t="s">
+      <c r="B3" s="28"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="13" t="s">
         <v>23</v>
       </c>
       <c r="F3" s="8"/>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="J3" s="17"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="17"/>
-    </row>
-    <row r="4" ht="140" spans="1:12">
+      <c r="I3" s="13"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="13"/>
+    </row>
+    <row r="4" spans="1:11" ht="135" x14ac:dyDescent="0.15">
       <c r="A4" s="8">
         <v>3</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="19"/>
-      <c r="D4" s="14" t="s">
+      <c r="B4" s="29"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="13" t="s">
         <v>25</v>
       </c>
       <c r="F4" s="8"/>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="17"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="17"/>
-    </row>
-    <row r="5" ht="84" spans="1:12">
-      <c r="A5" s="20">
+      <c r="I4" s="13"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="13"/>
+    </row>
+    <row r="5" spans="1:11" ht="81" x14ac:dyDescent="0.15">
+      <c r="A5" s="14">
         <v>4</v>
       </c>
-      <c r="B5" s="21">
+      <c r="B5" s="27">
         <v>196110130</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="23" t="s">
+      <c r="E5" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20" t="s">
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="15"/>
+    </row>
+    <row r="6" spans="1:11" ht="81" x14ac:dyDescent="0.15">
+      <c r="A6" s="14">
+        <v>5</v>
+      </c>
+      <c r="B6" s="28"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="23"/>
-    </row>
-    <row r="6" ht="84" spans="1:12">
-      <c r="A6" s="20">
-        <v>5</v>
-      </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="25"/>
-      <c r="D6" s="23" t="s">
+      <c r="E6" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="15"/>
+    </row>
+    <row r="7" spans="1:11" ht="94.5" x14ac:dyDescent="0.15">
+      <c r="A7" s="14">
+        <v>6</v>
+      </c>
+      <c r="B7" s="28"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="23" t="s">
+      <c r="E7" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="20"/>
-      <c r="G6" s="20" t="s">
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="15"/>
+    </row>
+    <row r="8" spans="1:11" ht="94.5" x14ac:dyDescent="0.15">
+      <c r="A8" s="14">
+        <v>7</v>
+      </c>
+      <c r="B8" s="29"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="23"/>
-    </row>
-    <row r="7" ht="112" spans="1:12">
-      <c r="A7" s="20">
-        <v>6</v>
-      </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="23" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="23" t="s">
+      <c r="E8" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="20"/>
-      <c r="G7" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="20"/>
-      <c r="I7" s="20"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="23"/>
-    </row>
-    <row r="8" ht="112" spans="1:12">
-      <c r="A8" s="20">
-        <v>7</v>
-      </c>
-      <c r="B8" s="26"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="23" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="20"/>
-      <c r="G8" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="20"/>
-      <c r="I8" s="20"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="20"/>
-      <c r="L8" s="23"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="15"/>
     </row>
   </sheetData>
-  <autoFilter ref="I1">
-    <extLst/>
-  </autoFilter>
+  <autoFilter ref="H1"/>
   <mergeCells count="4">
     <mergeCell ref="B2:B4"/>
     <mergeCell ref="B5:B8"/>
     <mergeCell ref="C2:C4"/>
     <mergeCell ref="C5:C8"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
-  <headerFooter/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="9.36363636363636" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.72727272727273" style="2" customWidth="1"/>
-    <col min="3" max="4" width="23.1272727272727" style="2" customWidth="1"/>
-    <col min="5" max="5" width="20.6272727272727" style="3" customWidth="1"/>
-    <col min="6" max="6" width="16.6272727272727" style="1" customWidth="1"/>
+    <col min="1" max="1" width="9.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.75" style="2" customWidth="1"/>
+    <col min="3" max="4" width="23.125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="20.625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="16.625" style="1" customWidth="1"/>
     <col min="7" max="7" width="20.5" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.0909090909091" customWidth="1"/>
-    <col min="9" max="9" width="19.1272727272727" style="4" customWidth="1"/>
-    <col min="10" max="10" width="17.8727272727273" style="4" customWidth="1"/>
-    <col min="11" max="11" width="17.8727272727273" customWidth="1"/>
+    <col min="8" max="8" width="13.125" customWidth="1"/>
+    <col min="9" max="9" width="19.125" style="4" customWidth="1"/>
+    <col min="10" max="10" width="17.875" style="4" customWidth="1"/>
+    <col min="11" max="11" width="17.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A1" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>1</v>
@@ -1695,26 +1029,26 @@
         <v>15</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E1" s="6" t="s">
         <v>17</v>
       </c>
       <c r="F1" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="H1" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>38</v>
-      </c>
       <c r="J1"/>
     </row>
-    <row r="2" customHeight="1" spans="1:10">
+    <row r="2" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -1726,7 +1060,7 @@
       <c r="I2" s="8"/>
       <c r="J2"/>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
@@ -1738,7 +1072,7 @@
       <c r="I3" s="8"/>
       <c r="J3"/>
     </row>
-    <row r="4" ht="15" customHeight="1" spans="1:10">
+    <row r="4" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
@@ -1750,7 +1084,7 @@
       <c r="I4" s="8"/>
       <c r="J4"/>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A5" s="8"/>
       <c r="B5" s="8"/>
       <c r="C5" s="8"/>
@@ -1762,7 +1096,7 @@
       <c r="I5" s="8"/>
       <c r="J5"/>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A6" s="8"/>
       <c r="B6" s="8"/>
       <c r="C6" s="8"/>
@@ -1774,7 +1108,7 @@
       <c r="I6" s="8"/>
       <c r="J6"/>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A7" s="8"/>
       <c r="B7" s="8"/>
       <c r="C7" s="8"/>
@@ -1786,7 +1120,7 @@
       <c r="I7" s="8"/>
       <c r="J7"/>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A8" s="8"/>
       <c r="B8" s="8"/>
       <c r="C8" s="8"/>
@@ -1798,7 +1132,7 @@
       <c r="I8" s="8"/>
       <c r="J8"/>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A9" s="8"/>
       <c r="B9" s="8"/>
       <c r="C9" s="8"/>
@@ -1810,7 +1144,7 @@
       <c r="I9" s="8"/>
       <c r="J9"/>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A10" s="8"/>
       <c r="B10" s="8"/>
       <c r="C10" s="8"/>
@@ -1822,7 +1156,7 @@
       <c r="I10" s="8"/>
       <c r="J10"/>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
@@ -1834,7 +1168,7 @@
       <c r="I11" s="8"/>
       <c r="J11"/>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A12"/>
       <c r="B12"/>
       <c r="C12"/>
@@ -1845,7 +1179,7 @@
       <c r="I12"/>
       <c r="J12"/>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A13"/>
       <c r="B13"/>
       <c r="C13"/>
@@ -1856,7 +1190,7 @@
       <c r="I13"/>
       <c r="J13"/>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14"/>
       <c r="B14"/>
       <c r="C14"/>
@@ -1867,7 +1201,7 @@
       <c r="I14"/>
       <c r="J14"/>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
@@ -1878,7 +1212,7 @@
       <c r="I15"/>
       <c r="J15"/>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16"/>
@@ -1889,7 +1223,7 @@
       <c r="I16"/>
       <c r="J16"/>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17"/>
@@ -1900,7 +1234,7 @@
       <c r="I17"/>
       <c r="J17"/>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A18"/>
       <c r="B18"/>
       <c r="C18"/>
@@ -1911,7 +1245,7 @@
       <c r="I18"/>
       <c r="J18"/>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A19"/>
       <c r="B19"/>
       <c r="C19"/>
@@ -1922,7 +1256,7 @@
       <c r="I19"/>
       <c r="J19"/>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20"/>
@@ -1933,7 +1267,7 @@
       <c r="I20"/>
       <c r="J20"/>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
@@ -1944,7 +1278,7 @@
       <c r="I21"/>
       <c r="J21"/>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
@@ -1955,7 +1289,7 @@
       <c r="I22"/>
       <c r="J22"/>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
@@ -1966,7 +1300,7 @@
       <c r="I23"/>
       <c r="J23"/>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
@@ -1977,7 +1311,7 @@
       <c r="I24"/>
       <c r="J24"/>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
@@ -1988,7 +1322,7 @@
       <c r="I25"/>
       <c r="J25"/>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A26"/>
       <c r="B26"/>
       <c r="C26"/>
@@ -1999,7 +1333,7 @@
       <c r="I26"/>
       <c r="J26"/>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A27"/>
       <c r="B27"/>
       <c r="C27"/>
@@ -2010,7 +1344,7 @@
       <c r="I27"/>
       <c r="J27"/>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A28"/>
       <c r="B28"/>
       <c r="C28"/>
@@ -2021,7 +1355,7 @@
       <c r="I28"/>
       <c r="J28"/>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A29"/>
       <c r="B29"/>
       <c r="C29"/>
@@ -2032,7 +1366,7 @@
       <c r="I29"/>
       <c r="J29"/>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A30"/>
       <c r="B30"/>
       <c r="C30"/>
@@ -2043,7 +1377,7 @@
       <c r="I30"/>
       <c r="J30"/>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A31"/>
       <c r="B31"/>
       <c r="C31"/>
@@ -2054,7 +1388,7 @@
       <c r="I31"/>
       <c r="J31"/>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A32"/>
       <c r="B32"/>
       <c r="C32"/>
@@ -2065,7 +1399,7 @@
       <c r="I32"/>
       <c r="J32"/>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A33"/>
       <c r="B33"/>
       <c r="C33"/>
@@ -2076,7 +1410,7 @@
       <c r="I33"/>
       <c r="J33"/>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A34"/>
       <c r="B34"/>
       <c r="C34"/>
@@ -2087,7 +1421,7 @@
       <c r="I34"/>
       <c r="J34"/>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A35"/>
       <c r="B35"/>
       <c r="C35"/>
@@ -2098,7 +1432,7 @@
       <c r="I35"/>
       <c r="J35"/>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A36"/>
       <c r="B36"/>
       <c r="C36"/>
@@ -2109,7 +1443,7 @@
       <c r="I36"/>
       <c r="J36"/>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A37"/>
       <c r="B37"/>
       <c r="C37"/>
@@ -2120,7 +1454,7 @@
       <c r="I37"/>
       <c r="J37"/>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A38"/>
       <c r="B38"/>
       <c r="C38"/>
@@ -2131,7 +1465,7 @@
       <c r="I38"/>
       <c r="J38"/>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A39"/>
       <c r="B39"/>
       <c r="C39"/>
@@ -2142,7 +1476,7 @@
       <c r="I39"/>
       <c r="J39"/>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A40"/>
       <c r="B40"/>
       <c r="C40"/>
@@ -2153,7 +1487,7 @@
       <c r="I40"/>
       <c r="J40"/>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A41"/>
       <c r="B41"/>
       <c r="C41"/>
@@ -2164,7 +1498,7 @@
       <c r="I41"/>
       <c r="J41"/>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A42"/>
       <c r="B42"/>
       <c r="C42"/>
@@ -2175,7 +1509,7 @@
       <c r="I42"/>
       <c r="J42"/>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A43"/>
       <c r="B43"/>
       <c r="C43"/>
@@ -2186,7 +1520,7 @@
       <c r="I43"/>
       <c r="J43"/>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A44"/>
       <c r="B44"/>
       <c r="C44"/>
@@ -2197,7 +1531,7 @@
       <c r="I44"/>
       <c r="J44"/>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A45"/>
       <c r="B45"/>
       <c r="C45"/>
@@ -2208,7 +1542,7 @@
       <c r="I45"/>
       <c r="J45"/>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A46"/>
       <c r="B46"/>
       <c r="C46"/>
@@ -2219,7 +1553,7 @@
       <c r="I46"/>
       <c r="J46"/>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A47"/>
       <c r="B47"/>
       <c r="C47"/>
@@ -2230,7 +1564,7 @@
       <c r="I47"/>
       <c r="J47"/>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A48"/>
       <c r="B48"/>
       <c r="C48"/>
@@ -2241,7 +1575,7 @@
       <c r="I48"/>
       <c r="J48"/>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A49"/>
       <c r="B49"/>
       <c r="C49"/>
@@ -2252,7 +1586,7 @@
       <c r="I49"/>
       <c r="J49"/>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A50"/>
       <c r="B50"/>
       <c r="C50"/>
@@ -2263,7 +1597,7 @@
       <c r="I50"/>
       <c r="J50"/>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A51"/>
       <c r="B51"/>
       <c r="C51"/>
@@ -2274,7 +1608,7 @@
       <c r="I51"/>
       <c r="J51"/>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A52" s="4"/>
       <c r="B52"/>
       <c r="C52"/>
@@ -2285,7 +1619,7 @@
       <c r="I52"/>
       <c r="J52"/>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A53" s="4"/>
       <c r="B53"/>
       <c r="C53"/>
@@ -2296,7 +1630,7 @@
       <c r="I53"/>
       <c r="J53"/>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A54" s="4"/>
       <c r="B54"/>
       <c r="C54"/>
@@ -2307,7 +1641,7 @@
       <c r="I54"/>
       <c r="J54"/>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A55" s="4"/>
       <c r="B55"/>
       <c r="C55"/>
@@ -2318,7 +1652,7 @@
       <c r="I55"/>
       <c r="J55"/>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A56" s="4"/>
       <c r="B56"/>
       <c r="C56"/>
@@ -2329,7 +1663,7 @@
       <c r="I56"/>
       <c r="J56"/>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A57" s="4"/>
       <c r="B57"/>
       <c r="C57"/>
@@ -2340,7 +1674,7 @@
       <c r="I57"/>
       <c r="J57"/>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A58" s="4"/>
       <c r="B58"/>
       <c r="C58"/>
@@ -2351,7 +1685,7 @@
       <c r="I58"/>
       <c r="J58"/>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A59" s="4"/>
       <c r="B59"/>
       <c r="C59"/>
@@ -2362,7 +1696,7 @@
       <c r="I59"/>
       <c r="J59"/>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A60" s="4"/>
       <c r="B60"/>
       <c r="C60"/>
@@ -2373,7 +1707,7 @@
       <c r="I60"/>
       <c r="J60"/>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A61" s="4"/>
       <c r="B61"/>
       <c r="C61"/>
@@ -2384,7 +1718,7 @@
       <c r="I61"/>
       <c r="J61"/>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A62" s="4"/>
       <c r="B62"/>
       <c r="C62"/>
@@ -2395,7 +1729,7 @@
       <c r="I62"/>
       <c r="J62"/>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A63" s="4"/>
       <c r="B63"/>
       <c r="C63"/>
@@ -2406,7 +1740,7 @@
       <c r="I63"/>
       <c r="J63"/>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A64" s="4"/>
       <c r="B64"/>
       <c r="C64"/>
@@ -2417,7 +1751,7 @@
       <c r="I64"/>
       <c r="J64"/>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A65" s="4"/>
       <c r="B65"/>
       <c r="C65"/>
@@ -2428,7 +1762,7 @@
       <c r="I65"/>
       <c r="J65"/>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A66" s="4"/>
       <c r="B66"/>
       <c r="C66"/>
@@ -2439,7 +1773,7 @@
       <c r="I66"/>
       <c r="J66"/>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A67" s="4"/>
       <c r="B67"/>
       <c r="C67"/>
@@ -2450,7 +1784,7 @@
       <c r="I67"/>
       <c r="J67"/>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A68" s="4"/>
       <c r="B68"/>
       <c r="C68"/>
@@ -2461,7 +1795,7 @@
       <c r="I68"/>
       <c r="J68"/>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A69" s="4"/>
       <c r="B69"/>
       <c r="C69"/>
@@ -2472,7 +1806,7 @@
       <c r="I69"/>
       <c r="J69"/>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A70" s="4"/>
       <c r="B70"/>
       <c r="C70"/>
@@ -2483,7 +1817,7 @@
       <c r="I70"/>
       <c r="J70"/>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A71" s="4"/>
       <c r="B71"/>
       <c r="C71"/>
@@ -2494,7 +1828,7 @@
       <c r="I71"/>
       <c r="J71"/>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A72" s="4"/>
       <c r="B72"/>
       <c r="C72"/>
@@ -2505,7 +1839,7 @@
       <c r="I72"/>
       <c r="J72"/>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A73" s="4"/>
       <c r="B73"/>
       <c r="C73"/>
@@ -2516,7 +1850,7 @@
       <c r="I73"/>
       <c r="J73"/>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A74" s="4"/>
       <c r="B74"/>
       <c r="C74"/>
@@ -2527,7 +1861,7 @@
       <c r="I74"/>
       <c r="J74"/>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A75" s="4"/>
       <c r="B75"/>
       <c r="C75"/>
@@ -2538,7 +1872,7 @@
       <c r="I75"/>
       <c r="J75"/>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A76" s="4"/>
       <c r="B76"/>
       <c r="C76"/>
@@ -2549,7 +1883,7 @@
       <c r="I76"/>
       <c r="J76"/>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A77" s="4"/>
       <c r="B77"/>
       <c r="C77"/>
@@ -2560,7 +1894,7 @@
       <c r="I77"/>
       <c r="J77"/>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A78" s="4"/>
       <c r="B78"/>
       <c r="C78"/>
@@ -2571,7 +1905,7 @@
       <c r="I78"/>
       <c r="J78"/>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A79" s="4"/>
       <c r="B79"/>
       <c r="C79"/>
@@ -2582,7 +1916,7 @@
       <c r="I79"/>
       <c r="J79"/>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A80" s="4"/>
       <c r="B80"/>
       <c r="C80"/>
@@ -2593,7 +1927,7 @@
       <c r="I80"/>
       <c r="J80"/>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A81" s="4"/>
       <c r="B81"/>
       <c r="C81"/>
@@ -2604,7 +1938,7 @@
       <c r="I81"/>
       <c r="J81"/>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A82" s="4"/>
       <c r="B82"/>
       <c r="C82"/>
@@ -2615,7 +1949,7 @@
       <c r="I82"/>
       <c r="J82"/>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A83" s="4"/>
       <c r="B83"/>
       <c r="C83"/>
@@ -2626,7 +1960,7 @@
       <c r="I83"/>
       <c r="J83"/>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A84" s="4"/>
       <c r="B84"/>
       <c r="C84"/>
@@ -2637,7 +1971,7 @@
       <c r="I84"/>
       <c r="J84"/>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A85" s="4"/>
       <c r="B85"/>
       <c r="C85"/>
@@ -2648,7 +1982,7 @@
       <c r="I85"/>
       <c r="J85"/>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A86" s="4"/>
       <c r="B86"/>
       <c r="C86"/>
@@ -2659,7 +1993,7 @@
       <c r="I86"/>
       <c r="J86"/>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A87" s="4"/>
       <c r="B87"/>
       <c r="C87"/>
@@ -2670,7 +2004,7 @@
       <c r="I87"/>
       <c r="J87"/>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A88" s="4"/>
       <c r="B88"/>
       <c r="C88"/>
@@ -2681,7 +2015,7 @@
       <c r="I88"/>
       <c r="J88"/>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A89" s="4"/>
       <c r="B89"/>
       <c r="C89"/>
@@ -2692,7 +2026,7 @@
       <c r="I89"/>
       <c r="J89"/>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A90" s="4"/>
       <c r="B90"/>
       <c r="C90"/>
@@ -2703,7 +2037,7 @@
       <c r="I90"/>
       <c r="J90"/>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A91" s="4"/>
       <c r="B91"/>
       <c r="C91"/>
@@ -2714,7 +2048,7 @@
       <c r="I91"/>
       <c r="J91"/>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A92" s="4"/>
       <c r="B92"/>
       <c r="C92"/>
@@ -2725,7 +2059,7 @@
       <c r="I92"/>
       <c r="J92"/>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A93" s="4"/>
       <c r="B93"/>
       <c r="C93"/>
@@ -2736,7 +2070,7 @@
       <c r="I93"/>
       <c r="J93"/>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A94" s="4"/>
       <c r="B94"/>
       <c r="C94"/>
@@ -2747,7 +2081,7 @@
       <c r="I94"/>
       <c r="J94"/>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A95" s="4"/>
       <c r="B95"/>
       <c r="C95"/>
@@ -2758,7 +2092,7 @@
       <c r="I95"/>
       <c r="J95"/>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A96" s="4"/>
       <c r="B96"/>
       <c r="C96"/>
@@ -2769,7 +2103,7 @@
       <c r="I96"/>
       <c r="J96"/>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A97" s="4"/>
       <c r="B97"/>
       <c r="C97"/>
@@ -2780,7 +2114,7 @@
       <c r="I97"/>
       <c r="J97"/>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A98" s="4"/>
       <c r="B98"/>
       <c r="C98"/>
@@ -2791,7 +2125,7 @@
       <c r="I98"/>
       <c r="J98"/>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A99" s="4"/>
       <c r="B99"/>
       <c r="C99"/>
@@ -2802,7 +2136,7 @@
       <c r="I99"/>
       <c r="J99"/>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A100" s="4"/>
       <c r="B100"/>
       <c r="C100"/>
@@ -2813,7 +2147,7 @@
       <c r="I100"/>
       <c r="J100"/>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A101" s="4"/>
       <c r="B101"/>
       <c r="C101"/>
@@ -2824,7 +2158,7 @@
       <c r="I101"/>
       <c r="J101"/>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A102" s="4"/>
       <c r="B102"/>
       <c r="C102"/>
@@ -2835,7 +2169,7 @@
       <c r="I102"/>
       <c r="J102"/>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A103" s="4"/>
       <c r="B103"/>
       <c r="C103"/>
@@ -2846,7 +2180,7 @@
       <c r="I103"/>
       <c r="J103"/>
     </row>
-    <row r="104" ht="16" customHeight="1" spans="1:10">
+    <row r="104" spans="1:10" ht="15.95" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A104" s="4"/>
       <c r="B104"/>
       <c r="C104"/>
@@ -2857,7 +2191,7 @@
       <c r="I104"/>
       <c r="J104"/>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A105" s="4"/>
       <c r="B105"/>
       <c r="C105"/>
@@ -2868,7 +2202,7 @@
       <c r="I105"/>
       <c r="J105"/>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A106" s="4"/>
       <c r="B106"/>
       <c r="C106"/>
@@ -2879,7 +2213,7 @@
       <c r="I106"/>
       <c r="J106"/>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A107" s="4"/>
       <c r="B107"/>
       <c r="C107"/>
@@ -2890,7 +2224,7 @@
       <c r="I107"/>
       <c r="J107"/>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A108" s="4"/>
       <c r="B108"/>
       <c r="C108"/>
@@ -2901,7 +2235,7 @@
       <c r="I108"/>
       <c r="J108"/>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A109" s="4"/>
       <c r="B109"/>
       <c r="C109"/>
@@ -2912,7 +2246,7 @@
       <c r="I109"/>
       <c r="J109"/>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A110" s="4"/>
       <c r="B110"/>
       <c r="C110"/>
@@ -2923,7 +2257,7 @@
       <c r="I110"/>
       <c r="J110"/>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A111" s="4"/>
       <c r="B111"/>
       <c r="C111"/>
@@ -2934,7 +2268,7 @@
       <c r="I111"/>
       <c r="J111"/>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A112" s="4"/>
       <c r="B112"/>
       <c r="C112"/>
@@ -2945,7 +2279,7 @@
       <c r="I112"/>
       <c r="J112"/>
     </row>
-    <row r="113" spans="1:10">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A113" s="4"/>
       <c r="B113"/>
       <c r="C113"/>
@@ -2956,7 +2290,7 @@
       <c r="I113"/>
       <c r="J113"/>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A114" s="4"/>
       <c r="B114"/>
       <c r="C114"/>
@@ -2967,7 +2301,7 @@
       <c r="I114"/>
       <c r="J114"/>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A115" s="4"/>
       <c r="B115"/>
       <c r="C115"/>
@@ -2978,7 +2312,7 @@
       <c r="I115"/>
       <c r="J115"/>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A116" s="4"/>
       <c r="B116"/>
       <c r="C116"/>
@@ -2989,7 +2323,7 @@
       <c r="I116"/>
       <c r="J116"/>
     </row>
-    <row r="117" spans="1:10">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A117" s="4"/>
       <c r="B117"/>
       <c r="C117"/>
@@ -3000,7 +2334,7 @@
       <c r="I117"/>
       <c r="J117"/>
     </row>
-    <row r="118" spans="1:10">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A118" s="4"/>
       <c r="B118"/>
       <c r="C118"/>
@@ -3011,7 +2345,7 @@
       <c r="I118"/>
       <c r="J118"/>
     </row>
-    <row r="119" spans="1:10">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A119" s="4"/>
       <c r="B119"/>
       <c r="C119"/>
@@ -3022,7 +2356,7 @@
       <c r="I119"/>
       <c r="J119"/>
     </row>
-    <row r="120" spans="1:10">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A120" s="4"/>
       <c r="B120"/>
       <c r="C120"/>
@@ -3033,7 +2367,7 @@
       <c r="I120"/>
       <c r="J120"/>
     </row>
-    <row r="121" spans="1:10">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A121" s="4"/>
       <c r="B121"/>
       <c r="C121"/>
@@ -3044,7 +2378,7 @@
       <c r="I121"/>
       <c r="J121"/>
     </row>
-    <row r="122" spans="1:10">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A122" s="4"/>
       <c r="B122"/>
       <c r="C122"/>
@@ -3055,7 +2389,7 @@
       <c r="I122"/>
       <c r="J122"/>
     </row>
-    <row r="123" spans="1:10">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A123" s="4"/>
       <c r="B123"/>
       <c r="C123"/>
@@ -3066,7 +2400,7 @@
       <c r="I123"/>
       <c r="J123"/>
     </row>
-    <row r="124" spans="1:10">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A124" s="4"/>
       <c r="B124"/>
       <c r="C124"/>
@@ -3077,7 +2411,7 @@
       <c r="I124"/>
       <c r="J124"/>
     </row>
-    <row r="125" spans="1:10">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A125" s="4"/>
       <c r="B125"/>
       <c r="C125"/>
@@ -3088,7 +2422,7 @@
       <c r="I125"/>
       <c r="J125"/>
     </row>
-    <row r="126" spans="1:10">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A126" s="4"/>
       <c r="B126"/>
       <c r="C126"/>
@@ -3099,7 +2433,7 @@
       <c r="I126"/>
       <c r="J126"/>
     </row>
-    <row r="127" spans="1:10">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A127" s="4"/>
       <c r="B127"/>
       <c r="C127"/>
@@ -3110,7 +2444,7 @@
       <c r="I127"/>
       <c r="J127"/>
     </row>
-    <row r="128" spans="1:10">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A128" s="4"/>
       <c r="B128"/>
       <c r="C128"/>
@@ -3121,7 +2455,7 @@
       <c r="I128"/>
       <c r="J128"/>
     </row>
-    <row r="129" spans="1:10">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A129" s="4"/>
       <c r="B129"/>
       <c r="C129"/>
@@ -3132,7 +2466,7 @@
       <c r="I129"/>
       <c r="J129"/>
     </row>
-    <row r="130" spans="1:10">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A130" s="4"/>
       <c r="B130"/>
       <c r="C130"/>
@@ -3143,7 +2477,7 @@
       <c r="I130"/>
       <c r="J130"/>
     </row>
-    <row r="131" spans="1:10">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A131" s="4"/>
       <c r="B131"/>
       <c r="C131"/>
@@ -3154,7 +2488,7 @@
       <c r="I131"/>
       <c r="J131"/>
     </row>
-    <row r="132" spans="1:10">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A132" s="4"/>
       <c r="B132"/>
       <c r="C132"/>
@@ -3165,7 +2499,7 @@
       <c r="I132"/>
       <c r="J132"/>
     </row>
-    <row r="133" spans="1:10">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A133" s="4"/>
       <c r="B133"/>
       <c r="C133"/>
@@ -3176,7 +2510,7 @@
       <c r="I133"/>
       <c r="J133"/>
     </row>
-    <row r="134" spans="1:10">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A134" s="4"/>
       <c r="B134"/>
       <c r="C134"/>
@@ -3187,7 +2521,7 @@
       <c r="I134"/>
       <c r="J134"/>
     </row>
-    <row r="135" spans="1:10">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A135" s="4"/>
       <c r="B135"/>
       <c r="C135"/>
@@ -3198,7 +2532,7 @@
       <c r="I135"/>
       <c r="J135"/>
     </row>
-    <row r="136" spans="1:10">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A136" s="4"/>
       <c r="B136"/>
       <c r="C136"/>
@@ -3209,7 +2543,7 @@
       <c r="I136"/>
       <c r="J136"/>
     </row>
-    <row r="137" spans="1:10">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A137" s="4"/>
       <c r="B137"/>
       <c r="C137"/>
@@ -3220,7 +2554,7 @@
       <c r="I137"/>
       <c r="J137"/>
     </row>
-    <row r="138" spans="1:10">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A138" s="4"/>
       <c r="B138"/>
       <c r="C138"/>
@@ -3231,7 +2565,7 @@
       <c r="I138"/>
       <c r="J138"/>
     </row>
-    <row r="139" spans="1:10">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A139" s="4"/>
       <c r="B139"/>
       <c r="C139"/>
@@ -3242,7 +2576,7 @@
       <c r="I139"/>
       <c r="J139"/>
     </row>
-    <row r="140" spans="1:10">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A140" s="4"/>
       <c r="B140"/>
       <c r="C140"/>
@@ -3253,7 +2587,7 @@
       <c r="I140"/>
       <c r="J140"/>
     </row>
-    <row r="141" spans="1:10">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A141" s="4"/>
       <c r="B141"/>
       <c r="C141"/>
@@ -3264,7 +2598,7 @@
       <c r="I141"/>
       <c r="J141"/>
     </row>
-    <row r="142" spans="1:10">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A142" s="4"/>
       <c r="B142"/>
       <c r="C142"/>
@@ -3275,7 +2609,7 @@
       <c r="I142"/>
       <c r="J142"/>
     </row>
-    <row r="143" spans="1:10">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A143" s="4"/>
       <c r="B143"/>
       <c r="C143"/>
@@ -3286,7 +2620,7 @@
       <c r="I143"/>
       <c r="J143"/>
     </row>
-    <row r="144" ht="18" customHeight="1" spans="1:10">
+    <row r="144" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A144" s="4"/>
       <c r="B144"/>
       <c r="C144"/>
@@ -3297,7 +2631,7 @@
       <c r="I144"/>
       <c r="J144"/>
     </row>
-    <row r="145" ht="18" customHeight="1" spans="1:10">
+    <row r="145" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A145" s="4"/>
       <c r="B145"/>
       <c r="C145"/>
@@ -3308,7 +2642,7 @@
       <c r="I145"/>
       <c r="J145"/>
     </row>
-    <row r="146" spans="1:10">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A146" s="4"/>
       <c r="B146"/>
       <c r="C146"/>
@@ -3319,7 +2653,7 @@
       <c r="I146"/>
       <c r="J146"/>
     </row>
-    <row r="147" spans="1:10">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A147" s="4"/>
       <c r="B147"/>
       <c r="C147"/>
@@ -3330,7 +2664,7 @@
       <c r="I147"/>
       <c r="J147"/>
     </row>
-    <row r="148" spans="1:10">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A148" s="4"/>
       <c r="B148"/>
       <c r="C148"/>
@@ -3341,7 +2675,7 @@
       <c r="I148"/>
       <c r="J148"/>
     </row>
-    <row r="149" spans="1:10">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A149" s="4"/>
       <c r="B149"/>
       <c r="C149"/>
@@ -3352,7 +2686,7 @@
       <c r="I149"/>
       <c r="J149"/>
     </row>
-    <row r="150" spans="1:10">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A150" s="4"/>
       <c r="B150"/>
       <c r="C150"/>
@@ -3363,7 +2697,7 @@
       <c r="I150"/>
       <c r="J150"/>
     </row>
-    <row r="151" spans="1:10">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A151" s="4"/>
       <c r="B151"/>
       <c r="C151"/>
@@ -3374,13 +2708,11 @@
       <c r="I151"/>
       <c r="J151"/>
     </row>
-    <row r="153" customHeight="1"/>
+    <row r="153" spans="1:10" ht="14.1" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <autoFilter ref="A1:J1">
-    <extLst/>
-  </autoFilter>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <autoFilter ref="A1:J1"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>